<commit_message>
Pequeños cambios en la memoria
Mirate el enunciado de la practica para ver si nos dejamos algo de la memoria.
</commit_message>
<xml_diff>
--- a/IAIC/Memoria IAIC/Comparativa ejemplos.xlsx
+++ b/IAIC/Memoria IAIC/Comparativa ejemplos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Universo1</t>
   </si>
@@ -63,13 +63,34 @@
     <t>Coste uniforme</t>
   </si>
   <si>
-    <t>Profundidad iterativa</t>
-  </si>
-  <si>
     <t>Búsquedas no informadas</t>
   </si>
   <si>
     <t>Búsquedas informadas</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>3 segs</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0 segs</t>
+  </si>
+  <si>
+    <t>2 segs</t>
+  </si>
+  <si>
+    <t>1 segs</t>
+  </si>
+  <si>
+    <t>Profundizacion iterativa</t>
   </si>
 </sst>
 </file>
@@ -386,66 +407,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -456,44 +417,71 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -510,43 +498,13 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF00B050"/>
+        <color auto="1"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -840,172 +798,279 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="1" max="1" width="0.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B3" s="20"/>
-      <c r="C3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B4" s="20"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="J4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
+      <c r="C5" s="9">
+        <v>766</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1420</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>967</v>
+      </c>
+      <c r="H5" s="10">
+        <v>2805</v>
+      </c>
+      <c r="I5" s="10">
+        <v>3229</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>695</v>
+      </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
+      <c r="C6" s="12">
+        <v>213</v>
+      </c>
+      <c r="D6" s="13">
+        <v>112</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>100</v>
+      </c>
+      <c r="G6" s="13">
+        <v>239</v>
+      </c>
+      <c r="H6" s="13">
+        <v>80</v>
+      </c>
+      <c r="I6" s="13">
+        <v>105</v>
+      </c>
+      <c r="J6" s="13">
+        <v>2</v>
+      </c>
+      <c r="K6" s="14">
+        <v>243</v>
+      </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="10"/>
+      <c r="C7" s="12">
+        <v>19</v>
+      </c>
+      <c r="D7" s="13">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="13">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13">
+        <v>116</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
+      <c r="C8" s="12">
+        <v>29</v>
+      </c>
+      <c r="D8" s="13">
+        <v>101</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="13">
+        <v>18</v>
+      </c>
+      <c r="H8" s="13">
+        <v>117</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="14">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="13"/>
+      <c r="C10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="24"/>
+      <c r="G18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1015,10 +1080,10 @@
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:K10">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>